<commit_message>
added title and updated filtering
</commit_message>
<xml_diff>
--- a/LocalWorkshopBarrierSummary.xlsx
+++ b/LocalWorkshopBarrierSummary.xlsx
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9AC674-8651-4DC4-A735-0DF02D3A231B}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E84" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H90"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>